<commit_message>
PRINT PDF OPTION INCLUDED
Using reportlab module
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sreer\OneDrive\Documents\Git-Projects\PayrollGenerator-EXEL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OFFICIAL\SIMPLEE PROJECTS\payroll-xlsx-main\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1FA9D3D-5B57-4309-B2EC-4EDAF57B5689}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
   <si>
     <t>Sreeram</t>
   </si>
@@ -42,12 +43,18 @@
   </si>
   <si>
     <t>23-23-2332</t>
+  </si>
+  <si>
+    <t>Manu</t>
+  </si>
+  <si>
+    <t>STAFF</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -77,10 +84,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -360,16 +366,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:O3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A2:O4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="P3" sqref="P3"/>
+    <sheetView tabSelected="1" zoomScale="66" workbookViewId="0">
+      <selection activeCell="Q9" sqref="Q9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="5" max="7" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.88671875" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" customWidth="1"/>
+    <col min="6" max="6" width="12.5546875" customWidth="1"/>
+    <col min="7" max="7" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
     <col min="9" max="13" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
@@ -396,28 +405,28 @@
       <c r="G2">
         <v>12313123</v>
       </c>
-      <c r="H2" s="2">
+      <c r="H2">
         <v>123123</v>
       </c>
-      <c r="I2" s="2">
+      <c r="I2">
         <v>1231233</v>
       </c>
-      <c r="J2" s="2">
+      <c r="J2">
         <v>12213</v>
       </c>
-      <c r="K2" s="2">
+      <c r="K2">
         <v>122123</v>
       </c>
-      <c r="L2" s="2">
+      <c r="L2">
         <v>12312</v>
       </c>
-      <c r="M2" s="2">
+      <c r="M2">
         <v>12123</v>
       </c>
-      <c r="N2" s="2">
+      <c r="N2">
         <v>1213</v>
       </c>
-      <c r="O2" s="2">
+      <c r="O2">
         <v>123</v>
       </c>
     </row>
@@ -466,6 +475,53 @@
       </c>
       <c r="O3">
         <v>766</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4">
+        <v>1013</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="1">
+        <v>44961</v>
+      </c>
+      <c r="F4" s="1">
+        <v>162063</v>
+      </c>
+      <c r="G4">
+        <v>5666009</v>
+      </c>
+      <c r="H4">
+        <v>67799</v>
+      </c>
+      <c r="I4">
+        <v>54444</v>
+      </c>
+      <c r="J4">
+        <v>676</v>
+      </c>
+      <c r="K4">
+        <v>7666</v>
+      </c>
+      <c r="L4">
+        <v>8999</v>
+      </c>
+      <c r="M4">
+        <v>788</v>
+      </c>
+      <c r="N4">
+        <v>89</v>
+      </c>
+      <c r="O4">
+        <v>988</v>
       </c>
     </row>
   </sheetData>

</xml_diff>